<commit_message>
Updated template file with versioning in README
</commit_message>
<xml_diff>
--- a/templates/methodsMetadataTemplateV0.1.xlsx
+++ b/templates/methodsMetadataTemplateV0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimely/Dropbox/TESTwork/ESS-DIVE/gasex/Docs for GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69325EFC-3F97-9E48-AB14-8728ED79BD6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5392B9B-C1AD-B549-99E6-693104AF210D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="1360" windowWidth="23740" windowHeight="13720" xr2:uid="{1B7B20DA-8791-C342-B4FE-841EE672613A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>Metadata variable</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changed validation rules to not prevent free text entry. Fixed typo in validation information. Updated instructions. </t>
+  </si>
+  <si>
+    <t>This is version V0.1</t>
   </si>
 </sst>
 </file>
@@ -686,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CC70AD-F9B7-034C-8760-6157F974A15D}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -731,17 +734,22 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>91</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>